<commit_message>
updatd View Register Navigation
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-ViewRegister.data.xlsx
+++ b/tests/artifact/data/UI-ViewRegister.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070" tabRatio="500"/>
+    <workbookView windowWidth="18350" windowHeight="6800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -30,12 +30,25 @@
     <definedName name="webcookie">'[1]#system'!$O$2:$O$8</definedName>
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="225">
   <si>
     <t>login.screen</t>
   </si>
@@ -154,13 +167,13 @@
     <t>username</t>
   </si>
   <si>
-    <t>crypt:d0a382ddd1185c583b59f4825423e1eae6eda68194ea3aa6</t>
+    <t>crypt:6dab1efafe436f246bfe392a2b64a16eb50f519d281360b3</t>
   </si>
   <si>
     <t>password</t>
   </si>
   <si>
-    <t>crypt:a778b096dd48a3e533c7f774e607425ec041ca57f192e5de</t>
+    <t>crypt:adf6a09e5bcb826fd8eb2abadefa5770b5bace8a2ad9388a</t>
   </si>
   <si>
     <t>button.submit</t>
@@ -454,7 +467,7 @@
     <t>Type.EnterValue</t>
   </si>
   <si>
-    <t>Purchase</t>
+    <t>Sale</t>
   </si>
   <si>
     <t>validate.FromDateBox</t>
@@ -484,13 +497,13 @@
     <t>From.DateValue</t>
   </si>
   <si>
-    <t>01-01-2023</t>
+    <t>01-04-2023</t>
   </si>
   <si>
     <t>To.DateValue</t>
   </si>
   <si>
-    <t>01-05-2024</t>
+    <t>31-03-2024</t>
   </si>
   <si>
     <t>Click.FromCalender</t>
@@ -551,17 +564,176 @@
   </si>
   <si>
     <t>3000</t>
+  </si>
+  <si>
+    <t>vr.No</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/div/table/thead/tr/th[1]/div</t>
+  </si>
+  <si>
+    <t>vr.Inv.No</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/div/table/thead/tr/th[2]/div</t>
+  </si>
+  <si>
+    <t>vr.Inv.Date</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/div/table/thead/tr/th[3]/div</t>
+  </si>
+  <si>
+    <t>vr.Customer</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/div/table/thead/tr/th[4]/div</t>
+  </si>
+  <si>
+    <t>vr.GSTIN</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/div/table/thead/tr/th[5]/div</t>
+  </si>
+  <si>
+    <t>vr.TIN</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/div/table/thead/tr/th[6]/div</t>
+  </si>
+  <si>
+    <t>vr.TaxFree</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/div/table/thead/tr/th[7]/div</t>
+  </si>
+  <si>
+    <t>vr.Taxable</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/div/table/thead/tr/th[8]/div</t>
+  </si>
+  <si>
+    <t>vr.GAmount</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/div/table/thead/tr/th[9]/div</t>
+  </si>
+  <si>
+    <t>vr.table.row.xpath</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/div/table/tbody/tr</t>
+  </si>
+  <si>
+    <t>vr.No.values</t>
+  </si>
+  <si>
+    <t>/td[1]</t>
+  </si>
+  <si>
+    <t>vr.Inv.No.values</t>
+  </si>
+  <si>
+    <t>/td[2]</t>
+  </si>
+  <si>
+    <t>vr.Inv.Date.values</t>
+  </si>
+  <si>
+    <t>/td[3]</t>
+  </si>
+  <si>
+    <t>vr.Customer.values</t>
+  </si>
+  <si>
+    <t>/td[4]</t>
+  </si>
+  <si>
+    <t>vr.GSTIN.values</t>
+  </si>
+  <si>
+    <t>/td[5]</t>
+  </si>
+  <si>
+    <t>vr.TIN.values</t>
+  </si>
+  <si>
+    <t>/td[6]</t>
+  </si>
+  <si>
+    <t>vr.TaxFree.values</t>
+  </si>
+  <si>
+    <t>/td[7]</t>
+  </si>
+  <si>
+    <t>vr.Taxable.values</t>
+  </si>
+  <si>
+    <t>/td[8]</t>
+  </si>
+  <si>
+    <t>vr.GAmount.values</t>
+  </si>
+  <si>
+    <t>/td[9]</t>
+  </si>
+  <si>
+    <t>type.searchValue</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/section[2]/div/input</t>
+  </si>
+  <si>
+    <t>Search.Values.Register</t>
+  </si>
+  <si>
+    <t>6/SL-24</t>
+  </si>
+  <si>
+    <t>present.search.values</t>
+  </si>
+  <si>
+    <t>//tbody[@role='rowgroup']/tr/td[2]/a</t>
+  </si>
+  <si>
+    <t>empty.search</t>
+  </si>
+  <si>
+    <t>invoice.link</t>
+  </si>
+  <si>
+    <t>//*[text()=' ${Search.Values.Register} ']</t>
+  </si>
+  <si>
+    <t>sales.Invoice.Number</t>
+  </si>
+  <si>
+    <t>//span[text()=' 6/SL-24 ']</t>
+  </si>
+  <si>
+    <t>viewRegister.button</t>
+  </si>
+  <si>
+    <t>//*[text()='View Vouchers']</t>
+  </si>
+  <si>
+    <t>voucher.presentvalues</t>
+  </si>
+  <si>
+    <t>//*[text()='Vouchers:']</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -608,28 +780,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -642,47 +809,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -697,46 +825,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -757,6 +871,64 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -767,85 +939,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -857,97 +1113,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -977,16 +1149,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1010,16 +1182,46 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1043,93 +1245,48 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1138,88 +1295,103 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1257,52 +1429,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1665,10 +1837,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C89"/>
+  <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>
@@ -1843,7 +2015,7 @@
       <c r="A21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2392,6 +2564,219 @@
       </c>
       <c r="B89" s="2" t="s">
         <v>171</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated View register navigation script
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-ViewRegister.data.xlsx
+++ b/tests/artifact/data/UI-ViewRegister.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070" tabRatio="500"/>
+    <workbookView windowWidth="18350" windowHeight="6800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -30,12 +30,25 @@
     <definedName name="webcookie">'[1]#system'!$O$2:$O$8</definedName>
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="225">
   <si>
     <t>login.screen</t>
   </si>
@@ -154,13 +167,13 @@
     <t>username</t>
   </si>
   <si>
-    <t>crypt:d0a382ddd1185c583b59f4825423e1eae6eda68194ea3aa6</t>
+    <t>crypt:6dab1efafe436f246bfe392a2b64a16eb50f519d281360b3</t>
   </si>
   <si>
     <t>password</t>
   </si>
   <si>
-    <t>crypt:a778b096dd48a3e533c7f774e607425ec041ca57f192e5de</t>
+    <t>crypt:adf6a09e5bcb826fd8eb2abadefa5770b5bace8a2ad9388a</t>
   </si>
   <si>
     <t>button.submit</t>
@@ -454,7 +467,7 @@
     <t>Type.EnterValue</t>
   </si>
   <si>
-    <t>Purchase</t>
+    <t>Sale</t>
   </si>
   <si>
     <t>validate.FromDateBox</t>
@@ -484,13 +497,13 @@
     <t>From.DateValue</t>
   </si>
   <si>
-    <t>01-01-2023</t>
+    <t>01-04-2023</t>
   </si>
   <si>
     <t>To.DateValue</t>
   </si>
   <si>
-    <t>01-05-2024</t>
+    <t>31-03-2024</t>
   </si>
   <si>
     <t>Click.FromCalender</t>
@@ -551,17 +564,176 @@
   </si>
   <si>
     <t>3000</t>
+  </si>
+  <si>
+    <t>vr.No</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/div/table/thead/tr/th[1]/div</t>
+  </si>
+  <si>
+    <t>vr.Inv.No</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/div/table/thead/tr/th[2]/div</t>
+  </si>
+  <si>
+    <t>vr.Inv.Date</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/div/table/thead/tr/th[3]/div</t>
+  </si>
+  <si>
+    <t>vr.Customer</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/div/table/thead/tr/th[4]/div</t>
+  </si>
+  <si>
+    <t>vr.GSTIN</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/div/table/thead/tr/th[5]/div</t>
+  </si>
+  <si>
+    <t>vr.TIN</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/div/table/thead/tr/th[6]/div</t>
+  </si>
+  <si>
+    <t>vr.TaxFree</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/div/table/thead/tr/th[7]/div</t>
+  </si>
+  <si>
+    <t>vr.Taxable</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/div/table/thead/tr/th[8]/div</t>
+  </si>
+  <si>
+    <t>vr.GAmount</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/div/table/thead/tr/th[9]/div</t>
+  </si>
+  <si>
+    <t>vr.table.row.xpath</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/div/table/tbody/tr</t>
+  </si>
+  <si>
+    <t>vr.No.values</t>
+  </si>
+  <si>
+    <t>/td[1]</t>
+  </si>
+  <si>
+    <t>vr.Inv.No.values</t>
+  </si>
+  <si>
+    <t>/td[2]</t>
+  </si>
+  <si>
+    <t>vr.Inv.Date.values</t>
+  </si>
+  <si>
+    <t>/td[3]</t>
+  </si>
+  <si>
+    <t>vr.Customer.values</t>
+  </si>
+  <si>
+    <t>/td[4]</t>
+  </si>
+  <si>
+    <t>vr.GSTIN.values</t>
+  </si>
+  <si>
+    <t>/td[5]</t>
+  </si>
+  <si>
+    <t>vr.TIN.values</t>
+  </si>
+  <si>
+    <t>/td[6]</t>
+  </si>
+  <si>
+    <t>vr.TaxFree.values</t>
+  </si>
+  <si>
+    <t>/td[7]</t>
+  </si>
+  <si>
+    <t>vr.Taxable.values</t>
+  </si>
+  <si>
+    <t>/td[8]</t>
+  </si>
+  <si>
+    <t>vr.GAmount.values</t>
+  </si>
+  <si>
+    <t>/td[9]</t>
+  </si>
+  <si>
+    <t>type.searchValue</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/section[2]/div/input</t>
+  </si>
+  <si>
+    <t>Search.Values.Register</t>
+  </si>
+  <si>
+    <t>6/SL-24</t>
+  </si>
+  <si>
+    <t>present.search.values</t>
+  </si>
+  <si>
+    <t>//tbody[@role='rowgroup']/tr/td[2]/a</t>
+  </si>
+  <si>
+    <t>empty.search</t>
+  </si>
+  <si>
+    <t>invoice.link</t>
+  </si>
+  <si>
+    <t>//*[text()=' ${Search.Values.Register} ']</t>
+  </si>
+  <si>
+    <t>sales.Invoice.Number</t>
+  </si>
+  <si>
+    <t>//span[text()=' 6/SL-24 ']</t>
+  </si>
+  <si>
+    <t>viewRegister.button</t>
+  </si>
+  <si>
+    <t>//*[text()='View Vouchers']</t>
+  </si>
+  <si>
+    <t>voucher.presentvalues</t>
+  </si>
+  <si>
+    <t>//*[text()='Vouchers:']</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -608,28 +780,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -642,47 +809,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -697,46 +825,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -757,6 +871,64 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -767,85 +939,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -857,97 +1113,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -977,16 +1149,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1010,16 +1182,46 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1043,93 +1245,48 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1138,88 +1295,103 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1257,52 +1429,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1665,10 +1837,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C89"/>
+  <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>
@@ -1843,7 +2015,7 @@
       <c r="A21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2392,6 +2564,219 @@
       </c>
       <c r="B89" s="2" t="s">
         <v>171</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>